<commit_message>
Ajouts : - Pleins de tests sur Xarray et pas de solution appart changer de methode et retourner sur la bibliothèque netCDF. Les données ne correspondent pas à ce qu'on veut faire sur panoply. - Données d'exemple pour essayer sur les fichiers netCDF
</commit_message>
<xml_diff>
--- a/data/doc_file_log.xlsx
+++ b/data/doc_file_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb3735da50722f06/BUT/STAGE/Dev_NetCDF/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_46B13E7774BCA71365171AC139E1C7AEE7BAF633" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E94F0DE-3F2C-49AB-A291-79EBD399EF8E}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="11_46B13E7774BCA71365171AC139E1C7AEE7BAF633" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02AD1531-65F9-428F-9961-DC6CFE16CD90}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -437,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1627"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1610" workbookViewId="0">
-      <selection activeCell="H1634" sqref="H1634"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>